<commit_message>
update title array 8c3e9fa342c642d29235b4e90fa866d15ccc5c06
</commit_message>
<xml_diff>
--- a/nr-add-lipids/ig/StructureDefinition-mesures-cholesterol-diagnostic-report.xlsx
+++ b/nr-add-lipids/ig/StructureDefinition-mesures-cholesterol-diagnostic-report.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1394" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1394" uniqueCount="357">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-10-30T13:57:24+00:00</t>
+    <t>2024-10-30T16:05:44+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -648,6 +648,15 @@
   </si>
   <si>
     <t>Not all terminology uses fit this general pattern. In some cases, models should not use CodeableConcept and use Coding directly and provide their own structure for managing text, codings, translations and the relationship between elements and pre- and post-coordination.</t>
+  </si>
+  <si>
+    <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
+  &lt;coding&gt;
+    &lt;system value="http://loinc.org"/&gt;
+    &lt;code value="57698-3"/&gt;
+    &lt;display value="Lipid panel with direct LDL - Serum or Plasma"/&gt;
+  &lt;/coding&gt;
+&lt;/valueCodeableConcept&gt;</t>
   </si>
   <si>
     <t>Codes that describe Diagnostic Reports.</t>
@@ -3166,7 +3175,7 @@
         <v>80</v>
       </c>
       <c r="S15" t="s" s="2">
-        <v>80</v>
+        <v>202</v>
       </c>
       <c r="T15" t="s" s="2">
         <v>80</v>
@@ -3184,10 +3193,10 @@
         <v>117</v>
       </c>
       <c r="Y15" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="Z15" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="AA15" t="s" s="2">
         <v>80</v>
@@ -3220,28 +3229,28 @@
         <v>103</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="AM15" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AN15" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" t="s" s="2">
@@ -3260,19 +3269,19 @@
         <v>91</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="N16" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="O16" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="P16" t="s" s="2">
         <v>80</v>
@@ -3321,7 +3330,7 @@
         <v>80</v>
       </c>
       <c r="AF16" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="AG16" t="s" s="2">
         <v>78</v>
@@ -3336,28 +3345,28 @@
         <v>170</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="AM16" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="AN16" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" t="s" s="2">
@@ -3376,19 +3385,19 @@
         <v>91</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="N17" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="O17" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="P17" t="s" s="2">
         <v>80</v>
@@ -3437,7 +3446,7 @@
         <v>80</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AG17" t="s" s="2">
         <v>78</v>
@@ -3452,28 +3461,28 @@
         <v>170</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AN17" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" t="s" s="2">
@@ -3492,19 +3501,19 @@
         <v>91</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="N18" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="O18" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="P18" t="s" s="2">
         <v>80</v>
@@ -3553,7 +3562,7 @@
         <v>80</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>78</v>
@@ -3568,28 +3577,28 @@
         <v>103</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" t="s" s="2">
@@ -3608,19 +3617,19 @@
         <v>91</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="N19" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="O19" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="P19" t="s" s="2">
         <v>80</v>
@@ -3669,7 +3678,7 @@
         <v>80</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>78</v>
@@ -3687,25 +3696,25 @@
         <v>80</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" t="s" s="2">
@@ -3724,19 +3733,19 @@
         <v>91</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="N20" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="O20" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="P20" t="s" s="2">
         <v>80</v>
@@ -3785,7 +3794,7 @@
         <v>80</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>78</v>
@@ -3800,28 +3809,28 @@
         <v>170</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" t="s" s="2">
@@ -3840,19 +3849,19 @@
         <v>91</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O21" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="P21" t="s" s="2">
         <v>80</v>
@@ -3901,7 +3910,7 @@
         <v>80</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>78</v>
@@ -3916,24 +3925,24 @@
         <v>170</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -3956,19 +3965,19 @@
         <v>80</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="N22" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="O22" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="P22" t="s" s="2">
         <v>80</v>
@@ -4017,7 +4026,7 @@
         <v>80</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>78</v>
@@ -4035,10 +4044,10 @@
         <v>80</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="AN22" t="s" s="2">
         <v>80</v>
@@ -4046,18 +4055,18 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G23" t="s" s="2">
         <v>79</v>
@@ -4072,19 +4081,19 @@
         <v>80</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="N23" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="O23" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="P23" t="s" s="2">
         <v>80</v>
@@ -4121,7 +4130,7 @@
         <v>80</v>
       </c>
       <c r="AB23" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="AC23" s="2"/>
       <c r="AD23" t="s" s="2">
@@ -4131,7 +4140,7 @@
         <v>144</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>78</v>
@@ -4149,10 +4158,10 @@
         <v>80</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AN23" t="s" s="2">
         <v>80</v>
@@ -4160,16 +4169,16 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C24" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D24" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" t="s" s="2">
@@ -4188,19 +4197,19 @@
         <v>80</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="O24" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="P24" t="s" s="2">
         <v>80</v>
@@ -4249,7 +4258,7 @@
         <v>80</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>78</v>
@@ -4267,10 +4276,10 @@
         <v>80</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AN24" t="s" s="2">
         <v>80</v>
@@ -4278,16 +4287,16 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C25" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D25" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" t="s" s="2">
@@ -4306,19 +4315,19 @@
         <v>80</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="O25" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="P25" t="s" s="2">
         <v>80</v>
@@ -4367,7 +4376,7 @@
         <v>80</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>78</v>
@@ -4385,10 +4394,10 @@
         <v>80</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AN25" t="s" s="2">
         <v>80</v>
@@ -4396,16 +4405,16 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C26" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D26" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" t="s" s="2">
@@ -4424,19 +4433,19 @@
         <v>80</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="O26" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="P26" t="s" s="2">
         <v>80</v>
@@ -4485,7 +4494,7 @@
         <v>80</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>78</v>
@@ -4503,10 +4512,10 @@
         <v>80</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>80</v>
@@ -4514,16 +4523,16 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C27" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D27" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" t="s" s="2">
@@ -4542,19 +4551,19 @@
         <v>80</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="O27" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="P27" t="s" s="2">
         <v>80</v>
@@ -4603,7 +4612,7 @@
         <v>80</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>78</v>
@@ -4621,10 +4630,10 @@
         <v>80</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AN27" t="s" s="2">
         <v>80</v>
@@ -4632,10 +4641,10 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -4658,16 +4667,16 @@
         <v>80</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="O28" s="2"/>
       <c r="P28" t="s" s="2">
@@ -4717,7 +4726,7 @@
         <v>80</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>78</v>
@@ -4738,7 +4747,7 @@
         <v>80</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>80</v>
@@ -4746,14 +4755,14 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" t="s" s="2">
@@ -4772,17 +4781,17 @@
         <v>91</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="P29" t="s" s="2">
         <v>80</v>
@@ -4831,7 +4840,7 @@
         <v>80</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>78</v>
@@ -4849,10 +4858,10 @@
         <v>80</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>80</v>
@@ -4860,10 +4869,10 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -4886,13 +4895,13 @@
         <v>80</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
@@ -4943,7 +4952,7 @@
         <v>80</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>78</v>
@@ -4972,10 +4981,10 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -5004,7 +5013,7 @@
         <v>139</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="N31" t="s" s="2">
         <v>141</v>
@@ -5057,7 +5066,7 @@
         <v>144</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>78</v>
@@ -5086,14 +5095,14 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" t="s" s="2">
@@ -5115,10 +5124,10 @@
         <v>138</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="N32" t="s" s="2">
         <v>141</v>
@@ -5173,7 +5182,7 @@
         <v>80</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>78</v>
@@ -5202,10 +5211,10 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5228,19 +5237,19 @@
         <v>80</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="O33" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="P33" t="s" s="2">
         <v>80</v>
@@ -5289,7 +5298,7 @@
         <v>80</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>78</v>
@@ -5310,7 +5319,7 @@
         <v>80</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>80</v>
@@ -5318,10 +5327,10 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5344,16 +5353,16 @@
         <v>91</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="N34" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="O34" s="2"/>
       <c r="P34" t="s" s="2">
@@ -5403,7 +5412,7 @@
         <v>80</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>90</v>
@@ -5424,7 +5433,7 @@
         <v>80</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="AN34" t="s" s="2">
         <v>80</v>
@@ -5432,14 +5441,14 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" t="s" s="2">
@@ -5458,19 +5467,19 @@
         <v>80</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="N35" t="s" s="2">
         <v>177</v>
       </c>
       <c r="O35" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="P35" t="s" s="2">
         <v>80</v>
@@ -5519,7 +5528,7 @@
         <v>80</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>78</v>
@@ -5537,10 +5546,10 @@
         <v>80</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>80</v>
@@ -5548,10 +5557,10 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -5577,10 +5586,10 @@
         <v>187</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="N36" t="s" s="2">
         <v>201</v>
@@ -5612,10 +5621,10 @@
         <v>191</v>
       </c>
       <c r="Y36" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="Z36" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="AA36" t="s" s="2">
         <v>80</v>
@@ -5633,7 +5642,7 @@
         <v>80</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>78</v>
@@ -5651,10 +5660,10 @@
         <v>80</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>80</v>
@@ -5662,10 +5671,10 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -5688,19 +5697,19 @@
         <v>80</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="N37" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="O37" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="P37" t="s" s="2">
         <v>80</v>
@@ -5749,7 +5758,7 @@
         <v>80</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>78</v>
@@ -5761,16 +5770,16 @@
         <v>102</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="AK37" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>80</v>

</xml_diff>